<commit_message>
Added keyword for week5 challenges
</commit_message>
<xml_diff>
--- a/questions/2018/5a_ak.xlsx
+++ b/questions/2018/5a_ak.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koji\OneDrive\Document\6th Form\pi\NCC_2018\questions\2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{C3354903-ACD7-45F0-9A86-68BE38489B4B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{36B3BFEC-330A-4400-B2A3-354B98BBB32E}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{C3354903-ACD7-45F0-9A86-68BE38489B4B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{E48F69CA-4BCA-468A-B6B8-C1C9ED03BD4F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8080" xr2:uid="{B3B5913D-D0F6-455E-A523-D7347F9AAFE5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>a</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>ariadne</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -726,7 +729,9 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.5">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>

</xml_diff>